<commit_message>
update view komite dan tambah fungsi ajax
</commit_message>
<xml_diff>
--- a/public/template/Impor Data Siswa.xlsx
+++ b/public/template/Impor Data Siswa.xlsx
@@ -53,16 +53,16 @@
     <t>12 MIA 2</t>
   </si>
   <si>
-    <t>06 jrf 0</t>
+    <t>55 kuh 7</t>
   </si>
   <si>
-    <t>06 wzy 0</t>
+    <t>16 tlf 5</t>
   </si>
   <si>
-    <t>08 ige 8</t>
+    <t>73 sxp 9</t>
   </si>
   <si>
-    <t>32 tdn 2</t>
+    <t>52 ngb 6</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
update proses store TahunAjaran baru
- add column nominal_daftar_ulang
- delete graduated siswa's komite
- reset komite when TahunAjaran is added
- formatting form nominal_daftar_ulang to rupiah and vice versa
</commit_message>
<xml_diff>
--- a/public/template/Impor Data Siswa.xlsx
+++ b/public/template/Impor Data Siswa.xlsx
@@ -53,16 +53,16 @@
     <t>12 MIA 2</t>
   </si>
   <si>
-    <t>55 kuh 7</t>
+    <t>79 min 5</t>
   </si>
   <si>
-    <t>16 tlf 5</t>
+    <t>26 epy 0</t>
   </si>
   <si>
-    <t>73 sxp 9</t>
+    <t>29 ngy 4</t>
   </si>
   <si>
-    <t>52 ngb 6</t>
+    <t>73 lwh 7</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
tambah fitur expor data komite
</commit_message>
<xml_diff>
--- a/public/template/Impor Data Siswa.xlsx
+++ b/public/template/Impor Data Siswa.xlsx
@@ -53,16 +53,16 @@
     <t>12 MIA 2</t>
   </si>
   <si>
-    <t>79 min 5</t>
+    <t>04 gbk 2</t>
   </si>
   <si>
-    <t>26 epy 0</t>
+    <t>19 kcy 3</t>
   </si>
   <si>
-    <t>29 ngy 4</t>
+    <t>27 jmy 6</t>
   </si>
   <si>
-    <t>73 lwh 7</t>
+    <t>56 pja 6</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
update delete pekerja function
</commit_message>
<xml_diff>
--- a/public/template/Impor Data Siswa.xlsx
+++ b/public/template/Impor Data Siswa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>SISTEM INFORMASI MANAJEMEN SMA NEGERI 5 MERANGIN</t>
   </si>
@@ -53,16 +53,10 @@
     <t>12 MIA 2</t>
   </si>
   <si>
-    <t>24 wao 6</t>
-  </si>
-  <si>
     <t>49 sbj 7</t>
   </si>
   <si>
     <t>45 iie 1</t>
-  </si>
-  <si>
-    <t>07 jig 7</t>
   </si>
 </sst>
 </file>
@@ -664,12 +658,8 @@
       <c r="F8" s="7"/>
       <c r="G8" s="11"/>
       <c r="H8" s="9"/>
-      <c r="J8" s="14">
-        <v>4</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" customHeight="1" ht="19.95">
       <c r="A9" s="7"/>
@@ -680,12 +670,8 @@
       <c r="F9" s="7"/>
       <c r="G9" s="11"/>
       <c r="H9" s="9"/>
-      <c r="J9" s="14">
-        <v>5</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" customHeight="1" ht="19.95">
       <c r="A10" s="7"/>

</xml_diff>